<commit_message>
upload file data kunjungan wisatawan mancanegara
</commit_message>
<xml_diff>
--- a/Jumlah Kunjungan Wisatawan Mancanegara per bulan ke Indonesia Menurut Pintu Masuk, 2017 - sekarang.xlsx
+++ b/Jumlah Kunjungan Wisatawan Mancanegara per bulan ke Indonesia Menurut Pintu Masuk, 2017 - sekarang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoga\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoga\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CEC574-83BF-4401-BD40-D863BF1FB117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46ED413-2CE8-43FC-BF02-C27138DFEE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="34">
   <si>
     <t>A. Pintu Udara</t>
   </si>
@@ -518,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH92"/>
+  <dimension ref="A1:AH89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="S100" sqref="S100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9779,318 +9779,6 @@
         <v>1066958</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
-        <v>45413</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" t="s">
-        <v>1</v>
-      </c>
-      <c r="E90" t="s">
-        <v>1</v>
-      </c>
-      <c r="F90" t="s">
-        <v>1</v>
-      </c>
-      <c r="G90" t="s">
-        <v>1</v>
-      </c>
-      <c r="H90" t="s">
-        <v>1</v>
-      </c>
-      <c r="I90" t="s">
-        <v>1</v>
-      </c>
-      <c r="J90" t="s">
-        <v>1</v>
-      </c>
-      <c r="K90" t="s">
-        <v>1</v>
-      </c>
-      <c r="L90" t="s">
-        <v>1</v>
-      </c>
-      <c r="M90" t="s">
-        <v>1</v>
-      </c>
-      <c r="N90" t="s">
-        <v>1</v>
-      </c>
-      <c r="O90" t="s">
-        <v>1</v>
-      </c>
-      <c r="P90" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>1</v>
-      </c>
-      <c r="R90" t="s">
-        <v>1</v>
-      </c>
-      <c r="S90" t="s">
-        <v>1</v>
-      </c>
-      <c r="T90" t="s">
-        <v>1</v>
-      </c>
-      <c r="U90" t="s">
-        <v>1</v>
-      </c>
-      <c r="V90" t="s">
-        <v>1</v>
-      </c>
-      <c r="W90" t="s">
-        <v>1</v>
-      </c>
-      <c r="X90" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y90" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG90" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH90" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
-        <v>45444</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" t="s">
-        <v>1</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1</v>
-      </c>
-      <c r="E91" t="s">
-        <v>1</v>
-      </c>
-      <c r="F91" t="s">
-        <v>1</v>
-      </c>
-      <c r="G91" t="s">
-        <v>1</v>
-      </c>
-      <c r="H91" t="s">
-        <v>1</v>
-      </c>
-      <c r="I91" t="s">
-        <v>1</v>
-      </c>
-      <c r="J91" t="s">
-        <v>1</v>
-      </c>
-      <c r="K91" t="s">
-        <v>1</v>
-      </c>
-      <c r="L91" t="s">
-        <v>1</v>
-      </c>
-      <c r="M91" t="s">
-        <v>1</v>
-      </c>
-      <c r="N91" t="s">
-        <v>1</v>
-      </c>
-      <c r="O91" t="s">
-        <v>1</v>
-      </c>
-      <c r="P91" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>1</v>
-      </c>
-      <c r="R91" t="s">
-        <v>1</v>
-      </c>
-      <c r="S91" t="s">
-        <v>1</v>
-      </c>
-      <c r="T91" t="s">
-        <v>1</v>
-      </c>
-      <c r="U91" t="s">
-        <v>1</v>
-      </c>
-      <c r="V91" t="s">
-        <v>1</v>
-      </c>
-      <c r="W91" t="s">
-        <v>1</v>
-      </c>
-      <c r="X91" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y91" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG91" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH91" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>45474</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" t="s">
-        <v>1</v>
-      </c>
-      <c r="D92" t="s">
-        <v>1</v>
-      </c>
-      <c r="E92" t="s">
-        <v>1</v>
-      </c>
-      <c r="F92" t="s">
-        <v>1</v>
-      </c>
-      <c r="G92" t="s">
-        <v>1</v>
-      </c>
-      <c r="H92" t="s">
-        <v>1</v>
-      </c>
-      <c r="I92" t="s">
-        <v>1</v>
-      </c>
-      <c r="J92" t="s">
-        <v>1</v>
-      </c>
-      <c r="K92" t="s">
-        <v>1</v>
-      </c>
-      <c r="L92" t="s">
-        <v>1</v>
-      </c>
-      <c r="M92" t="s">
-        <v>1</v>
-      </c>
-      <c r="N92" t="s">
-        <v>1</v>
-      </c>
-      <c r="O92" t="s">
-        <v>1</v>
-      </c>
-      <c r="P92" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>1</v>
-      </c>
-      <c r="R92" t="s">
-        <v>1</v>
-      </c>
-      <c r="S92" t="s">
-        <v>1</v>
-      </c>
-      <c r="T92" t="s">
-        <v>1</v>
-      </c>
-      <c r="U92" t="s">
-        <v>1</v>
-      </c>
-      <c r="V92" t="s">
-        <v>1</v>
-      </c>
-      <c r="W92" t="s">
-        <v>1</v>
-      </c>
-      <c r="X92" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y92" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AG92" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH92" t="s">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>